<commit_message>
Fehler in PDF und Excel von Rollen gefixt
(bei "bassist (instrumentalist))
</commit_message>
<xml_diff>
--- a/assets/documents/Digi-Kunst.nrw-Rollen-Grundset.xlsx
+++ b/assets/documents/Digi-Kunst.nrw-Rollen-Grundset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rene.Bialik\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rene.Bialik\Desktop\push\assets\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D2781D-FF04-4222-8DE9-2354B23F82D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A708966-0E58-4D23-9425-53A9B6D40ED4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28665" windowHeight="12045" xr2:uid="{70755527-EC53-4254-BE75-76AC39A24848}"/>
   </bookViews>
@@ -5280,8 +5280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EADB27AA-7C40-48B4-9B2D-F6EF1F453DEF}">
   <dimension ref="A1:N284"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A257" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D274" sqref="D274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12482,10 +12482,10 @@
         <v>1505</v>
       </c>
       <c r="C276" s="7"/>
-      <c r="D276" s="5" t="s">
+      <c r="D276" s="5"/>
+      <c r="E276" s="6" t="s">
         <v>1506</v>
       </c>
-      <c r="E276" s="6"/>
       <c r="F276" s="7"/>
       <c r="G276" s="8"/>
       <c r="H276" s="9" t="s">

</xml_diff>